<commit_message>
Update some apis to adapt active course, update data import excel
</commit_message>
<xml_diff>
--- a/excel/regulation-import.xlsx
+++ b/excel/regulation-import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\storage\sources\Web\2scool\2scool-api\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LEAT\data\src\others\2scool-api\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B93504-9864-4751-840D-F81DA65FA474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D525AF-7BDA-4882-9020-3AB795340928}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>STT</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>Học sinh</t>
+  </si>
+  <si>
+    <t>Mô tả</t>
+  </si>
+  <si>
+    <t>Mô tả 1</t>
+  </si>
+  <si>
+    <t>Mô tả 2</t>
   </si>
 </sst>
 </file>
@@ -378,69 +387,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="3" width="29.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>